<commit_message>
Added Supplementary Tables 4 and 5. removed superfluous files.
</commit_message>
<xml_diff>
--- a/data/manuscript_data/Supplementary Table 1.xlsx
+++ b/data/manuscript_data/Supplementary Table 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakegearon/CursorProjects/rulesofriveravulsion/data/manuscript_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakegearon/projects/rulesofriveravulsion/data/manuscript_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FFAA6B-9EF5-B14C-B4C4-2ADF66C6CF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255367CC-ECCB-F44D-88A1-66635FF3C66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="2260" windowWidth="17560" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,6 @@
     <t>geometry</t>
   </si>
   <si>
-    <t>dist_mtn_front_to_avulsion</t>
-  </si>
-  <si>
-    <t>total_transport distance</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -1106,6 +1100,12 @@
   </si>
   <si>
     <t>avulsion_name</t>
+  </si>
+  <si>
+    <t>total_transport distance (m)</t>
+  </si>
+  <si>
+    <t>dist_mtn_front_to_avulsion (m)</t>
   </si>
 </sst>
 </file>
@@ -1650,9 +1650,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1690,7 +1690,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1796,7 +1796,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1938,7 +1938,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1949,46 +1949,51 @@
   <dimension ref="A1:H175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>361</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>360</v>
       </c>
       <c r="E1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G1" t="s">
         <v>358</v>
       </c>
-      <c r="F1" t="s">
-        <v>359</v>
-      </c>
-      <c r="G1" t="s">
-        <v>360</v>
-      </c>
       <c r="H1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>14046</v>
@@ -2000,10 +2005,10 @@
         <v>0.51347102899999997</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2011,10 +2016,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>18421</v>
@@ -2026,10 +2031,10 @@
         <v>0.68517760800000005</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2037,10 +2042,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>18821</v>
@@ -2052,10 +2057,10 @@
         <v>0.70005579299999998</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2063,10 +2068,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>19221</v>
@@ -2078,10 +2083,10 @@
         <v>0.71493397800000003</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2089,10 +2094,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>13416</v>
@@ -2104,10 +2109,10 @@
         <v>0.47714905600000002</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2115,10 +2120,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>16940</v>
@@ -2130,10 +2135,10 @@
         <v>0.60248248400000004</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -2141,10 +2146,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>13725</v>
@@ -2156,10 +2161,10 @@
         <v>0.45569241999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -2167,10 +2172,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>13302</v>
@@ -2182,10 +2187,10 @@
         <v>0.42259427500000002</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -2193,10 +2198,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>16320</v>
@@ -2208,10 +2213,10 @@
         <v>0.51847380600000004</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -2219,10 +2224,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>10038</v>
@@ -2234,10 +2239,10 @@
         <v>3.371962E-3</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -2245,10 +2250,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>11532</v>
@@ -2260,10 +2265,10 @@
         <v>3.8738259999999999E-3</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2271,10 +2276,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>12986</v>
@@ -2286,10 +2291,10 @@
         <v>4.362253E-3</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2297,10 +2302,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>43940</v>
@@ -2312,10 +2317,10 @@
         <v>1.433126E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2323,10 +2328,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>47953</v>
@@ -2338,10 +2343,10 @@
         <v>1.564012E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2349,10 +2354,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>48420</v>
@@ -2364,10 +2369,10 @@
         <v>1.5792435000000001E-2</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2375,10 +2380,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17">
         <v>23710</v>
@@ -2390,10 +2395,10 @@
         <v>7.7343630000000002E-3</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2401,10 +2406,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18">
         <v>69653</v>
@@ -2416,10 +2421,10 @@
         <v>2.3606081000000001E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2427,10 +2432,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>8787</v>
@@ -2442,10 +2447,10 @@
         <v>2.8973169999999999E-3</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2453,10 +2458,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>10000</v>
@@ -2468,10 +2473,10 @@
         <v>3.261552E-3</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2479,10 +2484,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>19047</v>
@@ -2494,7 +2499,7 @@
         <v>5.9310949999999999E-3</v>
       </c>
       <c r="G21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2502,10 +2507,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>29612</v>
@@ -2517,10 +2522,10 @@
         <v>0.380959732</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2528,10 +2533,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>35031</v>
@@ -2543,10 +2548,10 @@
         <v>7.1815592999999997E-2</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2554,10 +2559,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>36270</v>
@@ -2569,10 +2574,10 @@
         <v>8.9465427E-2</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2580,10 +2585,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>7304</v>
@@ -2595,10 +2600,10 @@
         <v>0.77487799700000004</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -2606,10 +2611,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>12690</v>
@@ -2621,10 +2626,10 @@
         <v>0.42271818799999999</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2632,10 +2637,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27">
         <v>85812</v>
@@ -2647,10 +2652,10 @@
         <v>0.82053929999999997</v>
       </c>
       <c r="F27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2658,10 +2663,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28">
         <v>3739</v>
@@ -2673,10 +2678,10 @@
         <v>2.108427E-3</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2684,10 +2689,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29">
         <v>394459</v>
@@ -2699,10 +2704,10 @@
         <v>0.98925127599999996</v>
       </c>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2710,10 +2715,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30">
         <v>144786</v>
@@ -2725,10 +2730,10 @@
         <v>0.92758618500000001</v>
       </c>
       <c r="F30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -2736,10 +2741,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31">
         <v>67618</v>
@@ -2751,10 +2756,10 @@
         <v>0.97166259499999996</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -2762,10 +2767,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32">
         <v>14514</v>
@@ -2777,10 +2782,10 @@
         <v>0.76822103399999997</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -2788,10 +2793,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33">
         <v>91366</v>
@@ -2803,10 +2808,10 @@
         <v>0.96107967100000002</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -2814,10 +2819,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34">
         <v>100204</v>
@@ -2829,10 +2834,10 @@
         <v>0.98060399700000001</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -2840,10 +2845,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35">
         <v>101849</v>
@@ -2855,10 +2860,10 @@
         <v>0.961556254</v>
       </c>
       <c r="F35" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -2866,10 +2871,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36">
         <v>50561</v>
@@ -2881,10 +2886,10 @@
         <v>0.98440481300000005</v>
       </c>
       <c r="F36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2892,10 +2897,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <v>30417</v>
@@ -2907,10 +2912,10 @@
         <v>0.92503497400000001</v>
       </c>
       <c r="F37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -2918,10 +2923,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38">
         <v>4646</v>
@@ -2933,10 +2938,10 @@
         <v>0.42121486899999999</v>
       </c>
       <c r="F38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2944,10 +2949,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39">
         <v>7623</v>
@@ -2959,10 +2964,10 @@
         <v>8.0605590000000001E-3</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2970,10 +2975,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40">
         <v>15644</v>
@@ -2985,10 +2990,10 @@
         <v>0.65077582300000003</v>
       </c>
       <c r="F40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2996,10 +3001,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41">
         <v>39413</v>
@@ -3011,10 +3016,10 @@
         <v>0.92235145399999996</v>
       </c>
       <c r="F41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3022,10 +3027,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>45456</v>
@@ -3037,10 +3042,10 @@
         <v>0.85594848000000001</v>
       </c>
       <c r="F42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3048,10 +3053,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43">
         <v>6472</v>
@@ -3063,10 +3068,10 @@
         <v>0.57067277999999999</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3074,10 +3079,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44">
         <v>100945</v>
@@ -3089,10 +3094,10 @@
         <v>0.95948026799999997</v>
       </c>
       <c r="F44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3100,10 +3105,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45">
         <v>49396</v>
@@ -3115,10 +3120,10 @@
         <v>0.87824479099999997</v>
       </c>
       <c r="F45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3126,10 +3131,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46">
         <v>73852</v>
@@ -3141,10 +3146,10 @@
         <v>0.95935360700000005</v>
       </c>
       <c r="F46" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3152,10 +3157,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47">
         <v>90733</v>
@@ -3167,10 +3172,10 @@
         <v>0.94524372599999995</v>
       </c>
       <c r="F47" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3178,10 +3183,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48">
         <v>32865</v>
@@ -3193,10 +3198,10 @@
         <v>3.5520666999999999E-2</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -3204,10 +3209,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49">
         <v>5884</v>
@@ -3219,10 +3224,10 @@
         <v>0.72893954400000005</v>
       </c>
       <c r="F49" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3230,10 +3235,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50">
         <v>7149</v>
@@ -3245,10 +3250,10 @@
         <v>0.83069951200000003</v>
       </c>
       <c r="F50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3256,10 +3261,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51">
         <v>800</v>
@@ -3271,10 +3276,10 @@
         <v>1.060386E-3</v>
       </c>
       <c r="F51" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -3282,10 +3287,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52">
         <v>2885</v>
@@ -3297,10 +3302,10 @@
         <v>0.63658428899999997</v>
       </c>
       <c r="F52" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3308,10 +3313,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C53">
         <v>44632</v>
@@ -3323,10 +3328,10 @@
         <v>0.88703394499999999</v>
       </c>
       <c r="F53" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3334,10 +3339,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C54">
         <v>30025</v>
@@ -3349,10 +3354,10 @@
         <v>0.87185667</v>
       </c>
       <c r="F54" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3360,10 +3365,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C55">
         <v>6280</v>
@@ -3375,10 +3380,10 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="F55" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3386,10 +3391,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C56">
         <v>193151</v>
@@ -3401,10 +3406,10 @@
         <v>0.95312137600000002</v>
       </c>
       <c r="F56" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3412,10 +3417,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C57">
         <v>150987</v>
@@ -3427,10 +3432,10 @@
         <v>0.97407825599999998</v>
       </c>
       <c r="F57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G57" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3438,10 +3443,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C58">
         <v>29178</v>
@@ -3453,10 +3458,10 @@
         <v>0.92917648600000002</v>
       </c>
       <c r="F58" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G58" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -3464,10 +3469,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C59">
         <v>42756</v>
@@ -3479,10 +3484,10 @@
         <v>0.92397458600000004</v>
       </c>
       <c r="F59" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -3490,10 +3495,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C60">
         <v>32504</v>
@@ -3505,10 +3510,10 @@
         <v>0.88957004799999995</v>
       </c>
       <c r="F60" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3516,10 +3521,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C61">
         <v>34407</v>
@@ -3531,10 +3536,10 @@
         <v>0.94165138599999998</v>
       </c>
       <c r="F61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -3542,10 +3547,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C62">
         <v>33171</v>
@@ -3557,10 +3562,10 @@
         <v>0.93263418300000001</v>
       </c>
       <c r="F62" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -3568,10 +3573,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C63">
         <v>94201</v>
@@ -3583,10 +3588,10 @@
         <v>0.961764646</v>
       </c>
       <c r="F63" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -3594,10 +3599,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C64">
         <v>79212</v>
@@ -3609,10 +3614,10 @@
         <v>0.95647028999999995</v>
       </c>
       <c r="F64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -3620,10 +3625,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C65">
         <v>66640</v>
@@ -3635,10 +3640,10 @@
         <v>0.93839329699999996</v>
       </c>
       <c r="F65" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3646,10 +3651,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C66">
         <v>69403</v>
@@ -3661,10 +3666,10 @@
         <v>0.97031848600000004</v>
       </c>
       <c r="F66" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G66" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3672,10 +3677,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C67">
         <v>61178</v>
@@ -3687,10 +3692,10 @@
         <v>0.96626338599999995</v>
       </c>
       <c r="F67" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3698,10 +3703,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C68">
         <v>400471</v>
@@ -3713,10 +3718,10 @@
         <v>0.98408396200000003</v>
       </c>
       <c r="F68" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G68" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3724,10 +3729,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C69">
         <v>1472305</v>
@@ -3739,10 +3744,10 @@
         <v>0.99087133500000002</v>
       </c>
       <c r="F69" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G69" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3750,10 +3755,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C70">
         <v>330720</v>
@@ -3765,10 +3770,10 @@
         <v>0.97437378100000005</v>
       </c>
       <c r="F70" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G70" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -3776,10 +3781,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C71">
         <v>4080</v>
@@ -3791,10 +3796,10 @@
         <v>1.8582620000000001E-2</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -3802,10 +3807,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C72">
         <v>32038</v>
@@ -3817,10 +3822,10 @@
         <v>0.90880208799999995</v>
       </c>
       <c r="F72" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G72" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -3828,10 +3833,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C73">
         <v>18007</v>
@@ -3843,10 +3848,10 @@
         <v>0.88032265899999995</v>
       </c>
       <c r="F73" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G73" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -3854,10 +3859,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C74">
         <v>53679</v>
@@ -3869,10 +3874,10 @@
         <v>0.89545591000000002</v>
       </c>
       <c r="F74" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G74" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -3880,10 +3885,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C75">
         <v>16768</v>
@@ -3895,10 +3900,10 @@
         <v>0.78005210300000005</v>
       </c>
       <c r="F75" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3906,10 +3911,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B76" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C76">
         <v>3297</v>
@@ -3921,10 +3926,10 @@
         <v>0.61465324399999999</v>
       </c>
       <c r="F76" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G76" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3932,10 +3937,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B77" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C77">
         <v>3989</v>
@@ -3947,10 +3952,10 @@
         <v>0.56183098600000003</v>
       </c>
       <c r="F77" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G77" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3958,10 +3963,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B78" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C78">
         <v>8532</v>
@@ -3973,10 +3978,10 @@
         <v>0.76403689399999997</v>
       </c>
       <c r="F78" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G78" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -3984,10 +3989,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C79">
         <v>24589</v>
@@ -3999,10 +4004,10 @@
         <v>0.89460088800000004</v>
       </c>
       <c r="F79" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G79" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -4010,10 +4015,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B80" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C80">
         <v>1256</v>
@@ -4025,10 +4030,10 @@
         <v>1.8212928999999999E-2</v>
       </c>
       <c r="F80" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -4036,10 +4041,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C81">
         <v>5196</v>
@@ -4051,10 +4056,10 @@
         <v>0.50309837300000004</v>
       </c>
       <c r="F81" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G81" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -4062,10 +4067,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B82" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C82">
         <v>365634</v>
@@ -4077,10 +4082,10 @@
         <v>0.98647233999999995</v>
       </c>
       <c r="F82" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G82" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -4088,10 +4093,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B83" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C83">
         <v>729789</v>
@@ -4103,10 +4108,10 @@
         <v>0.99299531799999996</v>
       </c>
       <c r="F83" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G83" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -4114,10 +4119,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B84" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C84">
         <v>28809</v>
@@ -4129,10 +4134,10 @@
         <v>0.69821381000000005</v>
       </c>
       <c r="F84" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G84" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -4140,10 +4145,10 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B85" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C85">
         <v>33914</v>
@@ -4155,10 +4160,10 @@
         <v>0.83847998599999995</v>
       </c>
       <c r="F85" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G85" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -4166,10 +4171,10 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C86">
         <v>26404</v>
@@ -4181,10 +4186,10 @@
         <v>0.93834180300000003</v>
       </c>
       <c r="F86" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G86" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -4192,10 +4197,10 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B87" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C87">
         <v>540870</v>
@@ -4207,10 +4212,10 @@
         <v>0.98619541600000005</v>
       </c>
       <c r="F87" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G87" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -4218,10 +4223,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B88" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C88">
         <v>20824</v>
@@ -4233,10 +4238,10 @@
         <v>0.91493848899999997</v>
       </c>
       <c r="F88" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G88" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -4244,10 +4249,10 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B89" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C89">
         <v>62473</v>
@@ -4259,10 +4264,10 @@
         <v>0.95170848399999997</v>
       </c>
       <c r="F89" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G89" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -4270,10 +4275,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B90" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C90">
         <v>327607</v>
@@ -4285,10 +4290,10 @@
         <v>0.99181077299999998</v>
       </c>
       <c r="F90" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G90" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -4296,10 +4301,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B91" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C91">
         <v>205340</v>
@@ -4311,10 +4316,10 @@
         <v>0.95810897799999994</v>
       </c>
       <c r="F91" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G91" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -4322,10 +4327,10 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C92">
         <v>34270</v>
@@ -4337,10 +4342,10 @@
         <v>0.95168008900000001</v>
       </c>
       <c r="F92" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G92" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -4348,10 +4353,10 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B93" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C93">
         <v>35090</v>
@@ -4363,10 +4368,10 @@
         <v>0.97445154099999998</v>
       </c>
       <c r="F93" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G93" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -4374,10 +4379,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B94" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C94">
         <v>24190</v>
@@ -4389,10 +4394,10 @@
         <v>0.81011386500000004</v>
       </c>
       <c r="F94" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G94" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -4400,10 +4405,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B95" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C95">
         <v>52307</v>
@@ -4415,10 +4420,10 @@
         <v>0.72767869600000001</v>
       </c>
       <c r="F95" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G95" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -4426,10 +4431,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B96" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C96">
         <v>54387</v>
@@ -4441,10 +4446,10 @@
         <v>0.499531577</v>
       </c>
       <c r="F96" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G96" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -4452,10 +4457,10 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B97" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C97">
         <v>33481</v>
@@ -4467,10 +4472,10 @@
         <v>0.50590048499999996</v>
       </c>
       <c r="F97" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G97" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -4478,10 +4483,10 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B98" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C98">
         <v>59296</v>
@@ -4493,10 +4498,10 @@
         <v>0.68620893199999999</v>
       </c>
       <c r="F98" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G98" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -4504,10 +4509,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B99" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C99">
         <v>863606</v>
@@ -4519,10 +4524,10 @@
         <v>0.89098232300000002</v>
       </c>
       <c r="F99" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G99" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -4530,10 +4535,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B100" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C100">
         <v>643576</v>
@@ -4545,10 +4550,10 @@
         <v>0.66397736900000004</v>
       </c>
       <c r="F100" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G100" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H100">
         <v>0</v>
@@ -4556,10 +4561,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B101" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C101">
         <v>200062</v>
@@ -4571,10 +4576,10 @@
         <v>0.95273970600000002</v>
       </c>
       <c r="F101" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G101" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -4582,10 +4587,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B102" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C102">
         <v>7526</v>
@@ -4597,10 +4602,10 @@
         <v>2.0454929999999998E-3</v>
       </c>
       <c r="F102" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G102" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -4608,10 +4613,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B103" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C103">
         <v>23430</v>
@@ -4623,10 +4628,10 @@
         <v>1.1213268E-2</v>
       </c>
       <c r="F103" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G103" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -4634,10 +4639,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B104" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C104">
         <v>31560</v>
@@ -4649,10 +4654,10 @@
         <v>1.7210718E-2</v>
       </c>
       <c r="F104" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G104" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -4660,10 +4665,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B105" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C105">
         <v>29570</v>
@@ -4675,10 +4680,10 @@
         <v>1.930662E-2</v>
       </c>
       <c r="F105" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G105" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -4686,10 +4691,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B106" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C106">
         <v>77444</v>
@@ -4701,10 +4706,10 @@
         <v>5.0606971000000001E-2</v>
       </c>
       <c r="F106" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G106" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H106">
         <v>1</v>
@@ -4712,10 +4717,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B107" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C107">
         <v>10661</v>
@@ -4727,10 +4732,10 @@
         <v>7.2265569999999998E-3</v>
       </c>
       <c r="F107" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G107" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -4738,10 +4743,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C108">
         <v>12262</v>
@@ -4753,10 +4758,10 @@
         <v>8.4626449999999995E-3</v>
       </c>
       <c r="F108" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G108" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -4764,10 +4769,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B109" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C109">
         <v>8903</v>
@@ -4779,10 +4784,10 @@
         <v>6.1110419999999997E-3</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G109" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H109">
         <v>0</v>
@@ -4790,10 +4795,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B110" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C110">
         <v>90688</v>
@@ -4805,10 +4810,10 @@
         <v>6.0273987000000001E-2</v>
       </c>
       <c r="F110" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G110" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -4816,10 +4821,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B111" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C111">
         <v>5351</v>
@@ -4831,10 +4836,10 @@
         <v>3.6042750000000001E-3</v>
       </c>
       <c r="F111" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G111" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -4842,10 +4847,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B112" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C112">
         <v>967</v>
@@ -4857,10 +4862,10 @@
         <v>6.5134199999999996E-4</v>
       </c>
       <c r="F112" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G112" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -4868,10 +4873,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B113" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C113">
         <v>54254</v>
@@ -4883,10 +4888,10 @@
         <v>4.2725101000000001E-2</v>
       </c>
       <c r="F113" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G113" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -4894,10 +4899,10 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B114" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C114">
         <v>272652</v>
@@ -4909,10 +4914,10 @@
         <v>7.1691581000000004E-2</v>
       </c>
       <c r="F114" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G114" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -4920,10 +4925,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B115" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C115">
         <v>13062</v>
@@ -4935,10 +4940,10 @@
         <v>3.5886680000000002E-3</v>
       </c>
       <c r="F115" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G115" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H115">
         <v>1</v>
@@ -4946,10 +4951,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B116" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C116">
         <v>5510</v>
@@ -4961,10 +4966,10 @@
         <v>1.5138230000000001E-3</v>
       </c>
       <c r="F116" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G116" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -4972,10 +4977,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B117" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C117">
         <v>7101</v>
@@ -4987,10 +4992,10 @@
         <v>2.181115E-3</v>
       </c>
       <c r="F117" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G117" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H117">
         <v>1</v>
@@ -4998,10 +5003,10 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B118" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C118">
         <v>3395</v>
@@ -5013,10 +5018,10 @@
         <v>9.5659300000000005E-4</v>
       </c>
       <c r="F118" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G118" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -5024,10 +5029,10 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B119" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C119">
         <v>3122</v>
@@ -5039,10 +5044,10 @@
         <v>9.3969099999999999E-4</v>
       </c>
       <c r="F119" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G119" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -5050,10 +5055,10 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B120" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C120">
         <v>2236</v>
@@ -5065,10 +5070,10 @@
         <v>6.7301399999999999E-4</v>
       </c>
       <c r="F120" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G120" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H120">
         <v>0</v>
@@ -5076,10 +5081,10 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B121" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C121">
         <v>57327</v>
@@ -5091,10 +5096,10 @@
         <v>1.6421307999999999E-2</v>
       </c>
       <c r="F121" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G121" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H121">
         <v>1</v>
@@ -5102,10 +5107,10 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C122">
         <v>99648</v>
@@ -5117,10 +5122,10 @@
         <v>2.9993071E-2</v>
       </c>
       <c r="F122" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G122" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H122">
         <v>1</v>
@@ -5128,10 +5133,10 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B123" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C123">
         <v>22143</v>
@@ -5143,10 +5148,10 @@
         <v>6.6537640000000004E-3</v>
       </c>
       <c r="F123" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G123" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -5154,10 +5159,10 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B124" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C124">
         <v>54520</v>
@@ -5169,10 +5174,10 @@
         <v>1.6382747999999999E-2</v>
       </c>
       <c r="F124" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G124" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -5180,10 +5185,10 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B125" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C125">
         <v>13455</v>
@@ -5195,10 +5200,10 @@
         <v>3.7585330000000001E-3</v>
       </c>
       <c r="F125" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G125" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -5206,10 +5211,10 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B126" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C126">
         <v>168842</v>
@@ -5221,10 +5226,10 @@
         <v>4.9329744000000002E-2</v>
       </c>
       <c r="F126" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G126" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H126">
         <v>1</v>
@@ -5232,10 +5237,10 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B127" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C127">
         <v>19390</v>
@@ -5247,10 +5252,10 @@
         <v>9.1396819999999997E-3</v>
       </c>
       <c r="F127" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G127" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -5258,10 +5263,10 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B128" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C128">
         <v>18875</v>
@@ -5273,10 +5278,10 @@
         <v>0.755</v>
       </c>
       <c r="F128" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G128" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H128">
         <v>1</v>
@@ -5284,10 +5289,10 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B129" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C129">
         <v>17384</v>
@@ -5299,10 +5304,10 @@
         <v>1.5485066E-2</v>
       </c>
       <c r="F129" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G129" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H129">
         <v>0</v>
@@ -5310,10 +5315,10 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B130" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C130">
         <v>6853</v>
@@ -5325,10 +5330,10 @@
         <v>6.1449369999999996E-3</v>
       </c>
       <c r="F130" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G130" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H130">
         <v>0</v>
@@ -5336,10 +5341,10 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B131" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C131">
         <v>4154</v>
@@ -5351,10 +5356,10 @@
         <v>0.13871635600000001</v>
       </c>
       <c r="F131" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G131" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -5362,10 +5367,10 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B132" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C132">
         <v>11251</v>
@@ -5377,10 +5382,10 @@
         <v>5.4171610000000002E-3</v>
       </c>
       <c r="F132" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G132" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H132">
         <v>0</v>
@@ -5388,10 +5393,10 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B133" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C133">
         <v>19042</v>
@@ -5403,10 +5408,10 @@
         <v>1.4010753000000001E-2</v>
       </c>
       <c r="F133" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G133" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H133">
         <v>0</v>
@@ -5414,10 +5419,10 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B134" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C134">
         <v>65678</v>
@@ -5429,10 +5434,10 @@
         <v>0.198611972</v>
       </c>
       <c r="F134" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G134" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H134">
         <v>1</v>
@@ -5440,10 +5445,10 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B135" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C135">
         <v>8959</v>
@@ -5455,10 +5460,10 @@
         <v>3.8905487000000002E-2</v>
       </c>
       <c r="F135" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G135" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H135">
         <v>0</v>
@@ -5466,10 +5471,10 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B136" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C136">
         <v>1608</v>
@@ -5481,10 +5486,10 @@
         <v>1.5613317999999999E-2</v>
       </c>
       <c r="F136" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G136" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H136">
         <v>0</v>
@@ -5492,10 +5497,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B137" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C137">
         <v>4466</v>
@@ -5507,10 +5512,10 @@
         <v>4.3363854E-2</v>
       </c>
       <c r="F137" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G137" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H137">
         <v>0</v>
@@ -5518,10 +5523,10 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B138" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C138">
         <v>6344</v>
@@ -5533,10 +5538,10 @@
         <v>0.123225142</v>
       </c>
       <c r="F138" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G138" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H138">
         <v>0</v>
@@ -5544,10 +5549,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B139" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C139">
         <v>11527</v>
@@ -5559,10 +5564,10 @@
         <v>0.138734098</v>
       </c>
       <c r="F139" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G139" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H139">
         <v>1</v>
@@ -5570,10 +5575,10 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B140" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C140">
         <v>226</v>
@@ -5585,10 +5590,10 @@
         <v>2.7246309999999999E-3</v>
       </c>
       <c r="F140" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G140" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H140">
         <v>0</v>
@@ -5596,10 +5601,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B141" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C141">
         <v>26829</v>
@@ -5611,10 +5616,10 @@
         <v>0.32290249999999998</v>
       </c>
       <c r="F141" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G141" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H141">
         <v>0</v>
@@ -5622,10 +5627,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B142" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C142">
         <v>7527</v>
@@ -5637,10 +5642,10 @@
         <v>0.106817472</v>
       </c>
       <c r="F142" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G142" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H142">
         <v>1</v>
@@ -5648,10 +5653,10 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B143" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C143">
         <v>1416</v>
@@ -5663,10 +5668,10 @@
         <v>4.3517410000000001E-3</v>
       </c>
       <c r="F143" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G143" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H143">
         <v>0</v>
@@ -5674,10 +5679,10 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B144" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C144">
         <v>6767</v>
@@ -5689,10 +5694,10 @@
         <v>0.14002234699999999</v>
       </c>
       <c r="F144" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G144" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H144">
         <v>1</v>
@@ -5700,10 +5705,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B145" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C145">
         <v>6225</v>
@@ -5715,10 +5720,10 @@
         <v>0.48850349199999998</v>
       </c>
       <c r="F145" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G145" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H145">
         <v>0</v>
@@ -5726,10 +5731,10 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B146" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C146">
         <v>2445</v>
@@ -5741,10 +5746,10 @@
         <v>0.10016797099999999</v>
       </c>
       <c r="F146" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G146" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H146">
         <v>0</v>
@@ -5752,10 +5757,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B147" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C147">
         <v>2176</v>
@@ -5767,10 +5772,10 @@
         <v>0.146848428</v>
       </c>
       <c r="F147" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G147" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H147">
         <v>0</v>
@@ -5778,10 +5783,10 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B148" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C148">
         <v>10102</v>
@@ -5793,10 +5798,10 @@
         <v>0.71640309199999996</v>
       </c>
       <c r="F148" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G148" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H148">
         <v>0</v>
@@ -5804,10 +5809,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B149" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C149">
         <v>8914</v>
@@ -5819,10 +5824,10 @@
         <v>0.333370732</v>
       </c>
       <c r="F149" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G149" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H149">
         <v>0</v>
@@ -5830,10 +5835,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B150" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C150">
         <v>7739</v>
@@ -5845,10 +5850,10 @@
         <v>2.7554261E-2</v>
       </c>
       <c r="F150" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G150" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -5856,10 +5861,10 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B151" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C151">
         <v>31092</v>
@@ -5871,10 +5876,10 @@
         <v>0.11036607700000001</v>
       </c>
       <c r="F151" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G151" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H151">
         <v>0</v>
@@ -5882,10 +5887,10 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B152" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C152">
         <v>11044</v>
@@ -5897,10 +5902,10 @@
         <v>4.6763915000000003E-2</v>
       </c>
       <c r="F152" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G152" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H152">
         <v>1</v>
@@ -5908,10 +5913,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B153" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C153">
         <v>8735</v>
@@ -5923,10 +5928,10 @@
         <v>4.9983119999999999E-2</v>
       </c>
       <c r="F153" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G153" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H153">
         <v>0</v>
@@ -5934,10 +5939,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B154" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C154">
         <v>4737</v>
@@ -5949,10 +5954,10 @@
         <v>6.3957335000000004E-2</v>
       </c>
       <c r="F154" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G154" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H154">
         <v>0</v>
@@ -5960,10 +5965,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B155" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C155">
         <v>6914</v>
@@ -5975,10 +5980,10 @@
         <v>8.8637617000000002E-2</v>
       </c>
       <c r="F155" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G155" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H155">
         <v>0</v>
@@ -5986,10 +5991,10 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B156" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C156">
         <v>8562</v>
@@ -6001,10 +6006,10 @@
         <v>0.68748996299999998</v>
       </c>
       <c r="F156" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G156" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H156">
         <v>0</v>
@@ -6012,10 +6017,10 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B157" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C157">
         <v>4303</v>
@@ -6027,10 +6032,10 @@
         <v>0.34551148199999998</v>
       </c>
       <c r="F157" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G157" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -6038,10 +6043,10 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B158" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C158">
         <v>4866</v>
@@ -6053,10 +6058,10 @@
         <v>0.53279316799999998</v>
       </c>
       <c r="F158" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G158" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H158">
         <v>0</v>
@@ -6064,10 +6069,10 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B159" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C159">
         <v>42892</v>
@@ -6079,10 +6084,10 @@
         <v>2.3927990999999999E-2</v>
       </c>
       <c r="F159" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G159" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H159">
         <v>1</v>
@@ -6090,10 +6095,10 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B160" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C160">
         <v>9827</v>
@@ -6105,10 +6110,10 @@
         <v>4.3458220000000001E-3</v>
       </c>
       <c r="F160" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G160" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H160">
         <v>1</v>
@@ -6116,10 +6121,10 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B161" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C161">
         <v>6853</v>
@@ -6131,10 +6136,10 @@
         <v>6.1449369999999996E-3</v>
       </c>
       <c r="F161" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G161" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H161">
         <v>0</v>
@@ -6142,10 +6147,10 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B162" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C162">
         <v>14662</v>
@@ -6157,10 +6162,10 @@
         <v>1.2048747E-2</v>
       </c>
       <c r="F162" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G162" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H162">
         <v>1</v>
@@ -6168,10 +6173,10 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B163" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C163">
         <v>22181</v>
@@ -6183,10 +6188,10 @@
         <v>5.8999550000000001E-3</v>
       </c>
       <c r="F163" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G163" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H163">
         <v>0</v>
@@ -6194,10 +6199,10 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B164" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C164">
         <v>458588</v>
@@ -6209,10 +6214,10 @@
         <v>0.31649546299999998</v>
       </c>
       <c r="F164" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G164" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H164">
         <v>1</v>
@@ -6220,10 +6225,10 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B165" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C165">
         <v>1633453</v>
@@ -6235,10 +6240,10 @@
         <v>0.681967078</v>
       </c>
       <c r="F165" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G165" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H165">
         <v>0</v>
@@ -6246,10 +6251,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B166" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C166">
         <v>71113</v>
@@ -6261,10 +6266,10 @@
         <v>3.6347271E-2</v>
       </c>
       <c r="F166" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G166" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H166">
         <v>0</v>
@@ -6272,10 +6277,10 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B167" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C167">
         <v>1200</v>
@@ -6287,10 +6292,10 @@
         <v>6.7146000000000003E-4</v>
       </c>
       <c r="F167" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G167" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H167">
         <v>1</v>
@@ -6298,10 +6303,10 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B168" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C168">
         <v>6524</v>
@@ -6313,10 +6318,10 @@
         <v>4.9945110000000001E-3</v>
       </c>
       <c r="F168" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G168" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H168">
         <v>0</v>
@@ -6324,10 +6329,10 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B169" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C169">
         <v>18019</v>
@@ -6339,10 +6344,10 @@
         <v>1.1975972E-2</v>
       </c>
       <c r="F169" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G169" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H169">
         <v>0</v>
@@ -6350,10 +6355,10 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B170" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C170">
         <v>20589</v>
@@ -6365,10 +6370,10 @@
         <v>1.6086149000000001E-2</v>
       </c>
       <c r="F170" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G170" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H170">
         <v>0</v>
@@ -6376,10 +6381,10 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B171" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C171">
         <v>25161</v>
@@ -6391,10 +6396,10 @@
         <v>1.9658245000000001E-2</v>
       </c>
       <c r="F171" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G171" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H171">
         <v>0</v>
@@ -6402,10 +6407,10 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B172" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C172">
         <v>37557</v>
@@ -6417,10 +6422,10 @@
         <v>2.1015024E-2</v>
       </c>
       <c r="F172" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G172" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H172">
         <v>0</v>
@@ -6428,10 +6433,10 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B173" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C173">
         <v>44217</v>
@@ -6443,10 +6448,10 @@
         <v>2.5580281E-2</v>
       </c>
       <c r="F173" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G173" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H173">
         <v>0</v>
@@ -6454,10 +6459,10 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B174" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C174">
         <v>27325</v>
@@ -6469,10 +6474,10 @@
         <v>2.1125703999999999E-2</v>
       </c>
       <c r="F174" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G174" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H174">
         <v>0</v>
@@ -6480,10 +6485,10 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B175" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C175">
         <v>91321</v>
@@ -6495,10 +6500,10 @@
         <v>0.94248353900000004</v>
       </c>
       <c r="F175" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G175" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H175">
         <v>0</v>

</xml_diff>